<commit_message>
Front End Work Started
</commit_message>
<xml_diff>
--- a/quotes.xlsx
+++ b/quotes.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B101"/>
+  <dimension ref="A1:B261"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -448,1200 +448,4164 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>“The world as we have created it is a process of our thinking. It cannot be changed without changing our thinking.”</t>
+          <t xml:space="preserve">
+Toyota Passo  2018 X for Sale
+8.8/10
+</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Albert Einstein</t>
+          <t xml:space="preserve">
+                        PKR 37 lacs
+</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>“It is our choices, Harry, that show what we truly are, far more than our abilities.”</t>
+          <t xml:space="preserve">
+Toyota Corolla  2018 Altis Grande 1.8 for Sale
+8.1/10
+</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>J.K. Rowling</t>
+          <t xml:space="preserve">
+                        PKR 54 lacs
+</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>“There are only two ways to live your life. One is as though nothing is a miracle. The other is as though everything is a miracle.”</t>
+          <t xml:space="preserve">
+Toyota B B  2007  for Sale
+6.2/10
+</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Albert Einstein</t>
+          <t xml:space="preserve">
+                        PKR 18 lacs
+</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>“The person, be it gentleman or lady, who has not pleasure in a good novel, must be intolerably stupid.”</t>
+          <t xml:space="preserve">
+Toyota Vitz  2019 F 1.0 for Sale
+8.8/10
+</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Jane Austen</t>
+          <t xml:space="preserve">
+                        PKR 46 lacs
+</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>“Imperfection is beauty, madness is genius and it's better to be absolutely ridiculous than absolutely boring.”</t>
+          <t xml:space="preserve">
+Toyota Corolla  2017 GLi 1.3 VVTi for Sale
+</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Marilyn Monroe</t>
+          <t xml:space="preserve">
+                        PKR 37.25 lacs
+</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>“Try not to become a man of success. Rather become a man of value.”</t>
+          <t xml:space="preserve">
+Toyota Yaris  2020 ATIV CVT 1.3 for Sale
+</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Albert Einstein</t>
+          <t xml:space="preserve">
+                        PKR 40.5 lacs
+</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>“It is better to be hated for what you are than to be loved for what you are not.”</t>
+          <t xml:space="preserve">
+Toyota Aqua  2013 S for Sale
+</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>André Gide</t>
+          <t xml:space="preserve">
+                        PKR 32.65 lacs
+</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>“I have not failed. I've just found 10,000 ways that won't work.”</t>
+          <t xml:space="preserve">
+Toyota Corolla  2021 Altis X Automatic 1.6 for Sale
+</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Thomas A. Edison</t>
+          <t xml:space="preserve">
+                        PKR 55.5 lacs
+</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>“A woman is like a tea bag; you never know how strong it is until it's in hot water.”</t>
+          <t xml:space="preserve">
+Toyota Corolla  2016 Altis Grande CVT-i 1.8 for Sale
+</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Eleanor Roosevelt</t>
+          <t xml:space="preserve">
+                        PKR 41.35 lacs
+</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>“A day without sunshine is like, you know, night.”</t>
+          <t xml:space="preserve">
+Toyota Corolla  2023 Altis Grande X CVT-i 1.8 Black Interior for Sale
+</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Steve Martin</t>
+          <t xml:space="preserve">
+                        PKR 82.75 lacs
+</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>“This life is what you make it. No matter what, you're going to mess up sometimes, it's a universal truth. But the good part is you get to decide how you're going to mess it up. Girls will be your friends - they'll act like it anyway. But just remember, some come, some go. The ones that stay with you through everything - they're your true best friends. Don't let go of them. Also remember, sisters make the best friends in the world. As for lovers, well, they'll come and go too. And baby, I hate to say it, most of them - actually pretty much all of them are going to break your heart, but you can't give up because if you give up, you'll never find your soulmate. You'll never find that half who makes you whole and that goes for everything. Just because you fail once, doesn't mean you're gonna fail at everything. Keep trying, hold on, and always, always, always believe in yourself, because if you don't, then who will, sweetie? So keep your head high, keep your chin up, and most importantly, keep smiling, because life's a beautiful thing and there's so much to smile about.”</t>
+          <t xml:space="preserve">
+Toyota Vitz  2001 F 1.0 for Sale
+</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Marilyn Monroe</t>
+          <t xml:space="preserve">
+                        PKR 14.9 lacs
+</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>“It takes a great deal of bravery to stand up to our enemies, but just as much to stand up to our friends.”</t>
+          <t xml:space="preserve">
+Toyota Raize  2021 Z for Sale
+</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>J.K. Rowling</t>
+          <t xml:space="preserve">
+                        PKR 56.5 lacs
+</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>“If you can't explain it to a six year old, you don't understand it yourself.”</t>
+          <t xml:space="preserve">
+Toyota Corolla  2010 GLi 1.3 VVTi for Sale
+</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Albert Einstein</t>
+          <t xml:space="preserve">
+                        PKR 20.3 lacs
+</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>“You may not be her first, her last, or her only. She loved before she may love again. But if she loves you now, what else matters? She's not perfect—you aren't either, and the two of you may never be perfect together but if she can make you laugh, cause you to think twice, and admit to being human and making mistakes, hold onto her and give her the most you can. She may not be thinking about you every second of the day, but she will give you a part of her that she knows you can break—her heart. So don't hurt her, don't change her, don't analyze and don't expect more than she can give. Smile when she makes you happy, let her know when she makes you mad, and miss her when she's not there.”</t>
+          <t xml:space="preserve">
+Toyota Surf  2000 SSR-G 3.4 for Sale
+</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Bob Marley</t>
+          <t xml:space="preserve">
+                        PKR 33 lacs
+</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>“I like nonsense, it wakes up the brain cells. Fantasy is a necessary ingredient in living.”</t>
+          <t xml:space="preserve">
+Toyota Vitz  2008 B Intelligent Package 1.0 for Sale
+</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Dr. Seuss</t>
+          <t xml:space="preserve">
+                        PKR 16.8 lacs
+</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>“I may not have gone where I intended to go, but I think I have ended up where I needed to be.”</t>
+          <t xml:space="preserve">
+Toyota Vitz  2011  for Sale
+</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Douglas Adams</t>
+          <t xml:space="preserve">
+                        PKR 23.3 lacs
+</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>“The opposite of love is not hate, it's indifference. The opposite of art is not ugliness, it's indifference. The opposite of faith is not heresy, it's indifference. And the opposite of life is not death, it's indifference.”</t>
+          <t xml:space="preserve">
+Toyota Corolla  2012 XLi VVTi for Sale
+</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Elie Wiesel</t>
+          <t xml:space="preserve">
+                        PKR 21 lacs
+</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>“It is not a lack of love, but a lack of friendship that makes unhappy marriages.”</t>
+          <t xml:space="preserve">
+Toyota Corolla  2018 GLi Automatic 1.3 VVTi for Sale
+</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Friedrich Nietzsche</t>
+          <t xml:space="preserve">
+                        PKR 43 lacs
+</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>“Good friends, good books, and a sleepy conscience: this is the ideal life.”</t>
+          <t xml:space="preserve">
+Toyota Vitz  2013 F Limited 1.0 for Sale
+</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Mark Twain</t>
+          <t xml:space="preserve">
+                        PKR 26 lacs
+</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>“Life is what happens to us while we are making other plans.”</t>
+          <t xml:space="preserve">
+Toyota Yaris  2021 ATIV X CVT 1.5 for Sale
+</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Allen Saunders</t>
+          <t xml:space="preserve">
+                        PKR 45.75 lacs
+</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>“I love you without knowing how, or when, or from where. I love you simply, without problems or pride: I love you in this way because I do not know any other way of loving but this, in which there is no I or you, so intimate that your hand upon my chest is my hand, so intimate that when I fall asleep your eyes close.”</t>
+          <t xml:space="preserve">
+Toyota Corolla  2012 GLi Automatic 1.6 VVTi for Sale
+</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Pablo Neruda</t>
+          <t xml:space="preserve">
+                        PKR 26.9 lacs
+</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>“For every minute you are angry you lose sixty seconds of happiness.”</t>
+          <t xml:space="preserve">
+Toyota Platz  2004 F 1.0 for Sale
+</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Ralph Waldo Emerson</t>
+          <t xml:space="preserve">
+                        PKR 13.75 lacs
+</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>“If you judge people, you have no time to love them.”</t>
+          <t xml:space="preserve">
+Toyota Corolla  2013 XLi VVTi for Sale
+</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Mother Teresa</t>
+          <t xml:space="preserve">
+                        PKR 24 lacs
+</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>“Anyone who thinks sitting in church can make you a Christian must also think that sitting in a garage can make you a car.”</t>
+          <t xml:space="preserve">
+Toyota Corolla Indus 1998 GLi Special Edition 1.6 for Sale
+</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Garrison Keillor</t>
+          <t xml:space="preserve">
+                        PKR 16.35 lacs
+</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>“Beauty is in the eye of the beholder and it may be necessary from time to time to give a stupid or misinformed beholder a black eye.”</t>
+          <t xml:space="preserve">
+Toyota Vitz  2011 F M Package 1.0 for Sale
+</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Jim Henson</t>
+          <t xml:space="preserve">
+                        PKR 22.2 lacs
+</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>“Today you are You, that is truer than true. There is no one alive who is Youer than You.”</t>
+          <t xml:space="preserve">
+Toyota Corolla  2015 Altis Automatic 1.6 for Sale
+</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Dr. Seuss</t>
+          <t xml:space="preserve">
+                        PKR 36 lacs
+</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>“If you want your children to be intelligent, read them fairy tales. If you want them to be more intelligent, read them more fairy tales.”</t>
+          <t xml:space="preserve">
+Toyota Corolla  2015 GLi Automatic 1.3 VVTi for Sale
+</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Albert Einstein</t>
+          <t xml:space="preserve">
+                        PKR 30 lacs
+</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>“It is impossible to live without failing at something, unless you live so cautiously that you might as well not have lived at all - in which case, you fail by default.”</t>
+          <t xml:space="preserve">
+Toyota Aqua  2014 G LED Soft Leather Selection  for Sale
+</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>J.K. Rowling</t>
+          <t xml:space="preserve">
+                        PKR 37 lacs
+</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>“Logic will get you from A to Z; imagination will get you everywhere.”</t>
+          <t xml:space="preserve">
+Toyota Corolla  2021 Altis X Automatic 1.6 for Sale
+</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Albert Einstein</t>
+          <t xml:space="preserve">
+                        PKR 55.95 lacs
+</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>“One good thing about music, when it hits you, you feel no pain.”</t>
+          <t xml:space="preserve">
+Toyota Premio  2010 F EX Package 1.5 for Sale
+</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Bob Marley</t>
+          <t xml:space="preserve">
+                        PKR 41.75 lacs
+</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>“The more that you read, the more things you will know. The more that you learn, the more places you'll go.”</t>
+          <t xml:space="preserve">
+Toyota Allion  2006 A18 for Sale
+</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Dr. Seuss</t>
+          <t xml:space="preserve">
+                        PKR 23.5 lacs
+</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>“Of course it is happening inside your head, Harry, but why on earth should that mean that it is not real?”</t>
+          <t xml:space="preserve">
+Toyota Camry XV40 2007 G for Sale
+</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>J.K. Rowling</t>
+          <t xml:space="preserve">
+                        PKR 26.25 lacs
+</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>“The truth is, everyone is going to hurt you. You just got to find the ones worth suffering for.”</t>
+          <t xml:space="preserve">
+Toyota Corolla  2017 GLi 1.3 VVTi for Sale
+</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Bob Marley</t>
+          <t xml:space="preserve">
+                        PKR 37.25 lacs
+</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>“Not all of us can do great things. But we can do small things with great love.”</t>
+          <t xml:space="preserve">
+Toyota Platz  2003 F 1.0 for Sale
+</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Mother Teresa</t>
+          <t xml:space="preserve">
+                        PKR 12.5 lacs
+</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>“To the well-organized mind, death is but the next great adventure.”</t>
+          <t xml:space="preserve">
+Toyota Corolla  2018 GLi 1.3 VVTi for Sale
+</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>J.K. Rowling</t>
+          <t xml:space="preserve">
+                        PKR 38.5 lacs
+</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>“All you need is love. But a little chocolate now and then doesn't hurt.”</t>
+          <t xml:space="preserve">
+Toyota Corolla  2009 XLi VVTi for Sale
+</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Charles M. Schulz</t>
+          <t xml:space="preserve">
+                        PKR 21.8 lacs
+</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>“We read to know we're not alone.”</t>
+          <t xml:space="preserve">
+Toyota Corolla  1982  for Sale
+</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>William Nicholson</t>
+          <t xml:space="preserve">
+                        PKR 6.5 lacs
+</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>“Any fool can know. The point is to understand.”</t>
+          <t xml:space="preserve">
+Toyota Vitz  2010 B Intelligent Package 1.0 for Sale
+</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Albert Einstein</t>
+          <t xml:space="preserve">
+                        PKR 19.75 lacs
+</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>“I have always imagined that Paradise will be a kind of library.”</t>
+          <t xml:space="preserve">
+Toyota Corolla  2009 GLi 1.3 VVTi for Sale
+</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Jorge Luis Borges</t>
+          <t xml:space="preserve">
+                        PKR 20 lacs
+</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>“It is never too late to be what you might have been.”</t>
+          <t xml:space="preserve">
+Toyota Passo  2018 X S  for Sale
+</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>George Eliot</t>
+          <t xml:space="preserve">
+                        PKR 34.3 lacs
+</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>“A reader lives a thousand lives before he dies, said Jojen. The man who never reads lives only one.”</t>
+          <t xml:space="preserve">
+Toyota Passo  2013 X for Sale
+</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>George R.R. Martin</t>
+          <t xml:space="preserve">
+                        PKR 24.25 lacs
+</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>“You can never get a cup of tea large enough or a book long enough to suit me.”</t>
+          <t xml:space="preserve">
+Toyota Corolla  2014 GLi 1.3 VVTi for Sale
+</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>C.S. Lewis</t>
+          <t xml:space="preserve">
+                        PKR 29.5 lacs
+</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>“You believe lies so you eventually learn to trust no one but yourself.”</t>
+          <t xml:space="preserve">
+Toyota Corolla  2019 GLi Automatic 1.3 VVTi for Sale
+</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Marilyn Monroe</t>
+          <t xml:space="preserve">
+                        PKR 41.75 lacs
+</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>“If you can make a woman laugh, you can make her do anything.”</t>
+          <t xml:space="preserve">
+Toyota Corolla  2018 Altis Automatic 1.6 for Sale
+</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Marilyn Monroe</t>
+          <t xml:space="preserve">
+                        PKR 48.5 lacs
+</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>“Life is like riding a bicycle. To keep your balance, you must keep moving.”</t>
+          <t xml:space="preserve">
+Toyota Corolla  2018 Altis Automatic 1.6 for Sale
+</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Albert Einstein</t>
+          <t xml:space="preserve">
+                        PKR 47.5 lacs
+</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>“The real lover is the man who can thrill you by kissing your forehead or smiling into your eyes or just staring into space.”</t>
+          <t xml:space="preserve">
+Toyota Aqua  2014 G for Sale
+</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Marilyn Monroe</t>
+          <t xml:space="preserve">
+                        PKR 38.99 lacs
+</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>“A wise girl kisses but doesn't love, listens but doesn't believe, and leaves before she is left.”</t>
+          <t xml:space="preserve">
+Toyota Corolla  2015 GLi 1.3 VVTi for Sale
+</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Marilyn Monroe</t>
+          <t xml:space="preserve">
+                        PKR 35 lacs
+</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>“Only in the darkness can you see the stars.”</t>
+          <t xml:space="preserve">
+Toyota Passo  2009 G 1.0 for Sale
+</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Martin Luther King Jr.</t>
+          <t xml:space="preserve">
+                        PKR 16.75 lacs
+</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>“It matters not what someone is born, but what they grow to be.”</t>
+          <t xml:space="preserve">
+Toyota Yaris  2022 ATIV CVT 1.3 for Sale
+</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>J.K. Rowling</t>
+          <t xml:space="preserve">
+                        PKR 46 lacs
+</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>“Love does not begin and end the way we seem to think it does. Love is a battle, love is a war; love is a growing up.”</t>
+          <t xml:space="preserve">
+Toyota Corolla  2016 GLi Automatic 1.3 VVTi for Sale
+</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>James Baldwin</t>
+          <t xml:space="preserve">
+                        PKR 37.5 lacs
+</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>“There is nothing I would not do for those who are really my friends. I have no notion of loving people by halves, it is not my nature.”</t>
+          <t xml:space="preserve">
+Toyota Corolla  2021 Altis X Automatic 1.6 for Sale
+</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>Jane Austen</t>
+          <t xml:space="preserve">
+                        PKR 56.5 lacs
+</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>“Do one thing every day that scares you.”</t>
+          <t xml:space="preserve">
+Toyota Yaris  2020 ATIV CVT 1.3 for Sale
+</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>Eleanor Roosevelt</t>
+          <t xml:space="preserve">
+                        PKR 41.5 lacs
+</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>“I am good, but not an angel. I do sin, but I am not the devil. I am just a small girl in a big world trying to find someone to love.”</t>
+          <t xml:space="preserve">
+Toyota Sprinter  1987  for Sale
+</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>Marilyn Monroe</t>
+          <t xml:space="preserve">
+                        PKR 5 lacs
+</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>“If I were not a physicist, I would probably be a musician. I often think in music. I live my daydreams in music. I see my life in terms of music.”</t>
+          <t xml:space="preserve">
+Toyota Corolla  2015 Altis Automatic 1.6 for Sale
+</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>Albert Einstein</t>
+          <t xml:space="preserve">
+                        PKR 30.75 lacs
+</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>“If you only read the books that everyone else is reading, you can only think what everyone else is thinking.”</t>
+          <t xml:space="preserve">
+Toyota Aqua  2016 S for Sale
+</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>Haruki Murakami</t>
+          <t xml:space="preserve">
+                        PKR 46 lacs
+</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>“The difference between genius and stupidity is: genius has its limits.”</t>
+          <t xml:space="preserve">
+Toyota Aqua  2016  for Sale
+</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>Alexandre Dumas fils</t>
+          <t xml:space="preserve">
+                        PKR 48.5 lacs
+</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>“He's like a drug for you, Bella.”</t>
+          <t xml:space="preserve">
+Toyota Corolla Axio  2007 X 1.5 for Sale
+</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>Stephenie Meyer</t>
+          <t xml:space="preserve">
+                        PKR 26.75 lacs
+</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>“There is no friend as loyal as a book.”</t>
+          <t xml:space="preserve">
+Toyota Corolla 9th Generation 2004 SE Saloon Automatic for Sale
+</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>Ernest Hemingway</t>
+          <t xml:space="preserve">
+                        PKR 16 lacs
+</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>“When one door of happiness closes, another opens; but often we look so long at the closed door that we do not see the one which has been opened for us.”</t>
+          <t xml:space="preserve">
+Toyota Corolla  2013 XLi VVTi for Sale
+</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>Helen Keller</t>
+          <t xml:space="preserve">
+                        PKR 21.5 lacs
+</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>“Life isn't about finding yourself. Life is about creating yourself.”</t>
+          <t xml:space="preserve">
+Toyota Prius  2011 S 1.8 for Sale
+</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>George Bernard Shaw</t>
+          <t xml:space="preserve">
+                        PKR 38 lacs
+</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>“That's the problem with drinking, I thought, as I poured myself a drink. If something bad happens you drink in an attempt to forget; if something good happens you drink in order to celebrate; and if nothing happens you drink to make something happen.”</t>
+          <t xml:space="preserve">
+Toyota Vitz  2018 F 1.0 for Sale
+</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>Charles Bukowski</t>
+          <t xml:space="preserve">
+                        PKR 41.5 lacs
+</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>“You don’t forget the face of the person who was your last hope.”</t>
+          <t xml:space="preserve">
+Toyota Corolla  2022 Altis X Automatic 1.6 for Sale
+</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>Suzanne Collins</t>
+          <t xml:space="preserve">
+                        PKR 60 lacs
+</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>“Remember, we're madly in love, so it's all right to kiss me anytime you feel like it.”</t>
+          <t xml:space="preserve">
+Toyota Land Cruiser  1993 VX Limited 4.2D for Sale
+</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>Suzanne Collins</t>
+          <t xml:space="preserve">
+                        PKR 43.5 lacs
+</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>“To love at all is to be vulnerable. Love anything and your heart will be wrung and possibly broken. If you want to make sure of keeping it intact you must give it to no one, not even an animal. Wrap it carefully round with hobbies and little luxuries; avoid all entanglements. Lock it up safe in the casket or coffin of your selfishness. But in that casket, safe, dark, motionless, airless, it will change. It will not be broken; it will become unbreakable, impenetrable, irredeemable. To love is to be vulnerable.”</t>
+          <t xml:space="preserve">
+Toyota Corolla  2018 Altis Automatic 1.6 for Sale
+</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>C.S. Lewis</t>
+          <t xml:space="preserve">
+                        PKR 45.8 lacs
+</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>“Not all those who wander are lost.”</t>
+          <t xml:space="preserve">
+Toyota Corolla  2010 GLi 1.3 VVTi for Sale
+</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>J.R.R. Tolkien</t>
+          <t xml:space="preserve">
+                        PKR 19 lacs
+</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>“Do not pity the dead, Harry. Pity the living, and, above all those who live without love.”</t>
+          <t xml:space="preserve">
+Toyota Corolla  2018 XLi Automatic for Sale
+</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>J.K. Rowling</t>
+          <t xml:space="preserve">
+                        PKR 39.3 lacs
+</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>“There is nothing to writing. All you do is sit down at a typewriter and bleed.”</t>
+          <t xml:space="preserve">
+Toyota Corolla  2010 GLi 1.3 VVTi for Sale
+</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>Ernest Hemingway</t>
+          <t xml:space="preserve">
+                        PKR 21 lacs
+</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>“Finish each day and be done with it. You have done what you could. Some blunders and absurdities no doubt crept in; forget them as soon as you can. Tomorrow is a new day. You shall begin it serenely and with too high a spirit to be encumbered with your old nonsense.”</t>
+          <t xml:space="preserve">
+Toyota Prius  2013  for Sale
+</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>Ralph Waldo Emerson</t>
+          <t xml:space="preserve">
+                        PKR 43 lacs
+</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>“I have never let my schooling interfere with my education.”</t>
+          <t xml:space="preserve">
+Toyota Corolla 9th Generation 2004 SE Saloon Automatic for Sale
+</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>Mark Twain</t>
+          <t xml:space="preserve">
+                        PKR 15.5 lacs
+</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>“I have heard there are troubles of more than one kind. Some come from ahead and some come from behind. But I've bought a big bat. I'm all ready you see. Now my troubles are going to have troubles with me!”</t>
+          <t xml:space="preserve">
+Toyota Yaris  2020 ATIV CVT 1.3 for Sale
+</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>Dr. Seuss</t>
+          <t xml:space="preserve">
+                        PKR 40.5 lacs
+</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>“If I had a flower for every time I thought of you...I could walk through my garden forever.”</t>
+          <t xml:space="preserve">
+Toyota Prius  2013  for Sale
+</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>Alfred Tennyson</t>
+          <t xml:space="preserve">
+                        PKR 48 lacs
+</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>“Some people never go crazy. What truly horrible lives they must lead.”</t>
+          <t xml:space="preserve">
+Toyota Corolla  2019 Altis Automatic 1.6 for Sale
+</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>Charles Bukowski</t>
+          <t xml:space="preserve">
+                        PKR 52 lacs
+</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>“The trouble with having an open mind, of course, is that people will insist on coming along and trying to put things in it.”</t>
+          <t xml:space="preserve">
+Toyota Corolla  2018 Altis Automatic 1.6 for Sale
+</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>Terry Pratchett</t>
+          <t xml:space="preserve">
+                        PKR 45.5 lacs
+</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>“Think left and think right and think low and think high. Oh, the thinks you can think up if only you try!”</t>
+          <t xml:space="preserve">
+Toyota Land Cruiser  2017 ZX G-Frontier for Sale
+</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>Dr. Seuss</t>
+          <t xml:space="preserve">
+                        PKR 4.5 crore
+</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>“What really knocks me out is a book that, when you're all done reading it, you wish the author that wrote it was a terrific friend of yours and you could call him up on the phone whenever you felt like it. That doesn't happen much, though.”</t>
+          <t xml:space="preserve">
+Toyota Corolla  2022 Altis X Automatic 1.6 for Sale
+</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>J.D. Salinger</t>
+          <t xml:space="preserve">
+                        PKR 62 lacs
+</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>“The reason I talk to myself is because I’m the only one whose answers I accept.”</t>
+          <t xml:space="preserve">
+Toyota Corolla  2012 GLi Automatic 1.6 VVTi for Sale
+</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>George Carlin</t>
+          <t xml:space="preserve">
+                        PKR 26.9 lacs
+</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>“You may say I'm a dreamer, but I'm not the only one. I hope someday you'll join us. And the world will live as one.”</t>
+          <t xml:space="preserve">
+Toyota Aqua  2015 G LED Soft Leather Selection  for Sale
+</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>John Lennon</t>
+          <t xml:space="preserve">
+                        PKR 39.45 lacs
+</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>“I am free of all prejudice. I hate everyone equally. ”</t>
+          <t xml:space="preserve">
+Toyota Vitz  2020 F 1.0 for Sale
+</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>W.C. Fields</t>
+          <t xml:space="preserve">
+                        PKR 45.5 lacs
+</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>“The question isn't who is going to let me; it's who is going to stop me.”</t>
+          <t xml:space="preserve">
+Toyota Aqua  2018 S for Sale
+</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>Ayn Rand</t>
+          <t xml:space="preserve">
+                        PKR 45 lacs
+</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>“′Classic′ - a book which people praise and don't read.”</t>
+          <t xml:space="preserve">
+Toyota Corolla  2016 GLi Automatic 1.3 VVTi for Sale
+</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>Mark Twain</t>
+          <t xml:space="preserve">
+                        PKR 33.85 lacs
+</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>“Anyone who has never made a mistake has never tried anything new.”</t>
+          <t xml:space="preserve">
+Toyota Yaris Hatchback  2020  for Sale
+</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>Albert Einstein</t>
+          <t xml:space="preserve">
+                        PKR 46 lacs
+</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>“A lady's imagination is very rapid; it jumps from admiration to love, from love to matrimony in a moment.”</t>
+          <t xml:space="preserve">
+Toyota Corolla  2014 Altis SR Cruisetronic 1.6 for Sale
+</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>Jane Austen</t>
+          <t xml:space="preserve">
+                        PKR 38.75 lacs
+</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>“Remember, if the time should come when you have to make a choice between what is right and what is easy, remember what happened to a boy who was good, and kind, and brave, because he strayed across the path of Lord Voldemort. Remember Cedric Diggory.”</t>
+          <t xml:space="preserve">
+Toyota Vitz  2009 F 1.0 for Sale
+</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>J.K. Rowling</t>
+          <t xml:space="preserve">
+                        PKR 20.5 lacs
+</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>“I declare after all there is no enjoyment like reading! How much sooner one tires of any thing than of a book! -- When I have a house of my own, I shall be miserable if I have not an excellent library.”</t>
+          <t xml:space="preserve">
+Toyota Corolla  2019 GLi Automatic 1.3 VVTi for Sale
+</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>Jane Austen</t>
+          <t xml:space="preserve">
+                        PKR 61.2 lacs
+</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>“There are few people whom I really love, and still fewer of whom I think well. The more I see of the world, the more am I dissatisfied with it; and every day confirms my belief of the inconsistency of all human characters, and of the little dependence that can be placed on the appearance of merit or sense.”</t>
+          <t xml:space="preserve">
+Toyota Aqua  2015 G LED Soft Leather Selection  for Sale
+</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>Jane Austen</t>
+          <t xml:space="preserve">
+                        PKR 42.5 lacs
+</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>“Some day you will be old enough to start reading fairy tales again.”</t>
+          <t xml:space="preserve">
+Toyota Corolla  2022 Altis Grande X CVT-i 1.8 Black Interior for Sale
+</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>C.S. Lewis</t>
+          <t xml:space="preserve">
+                        PKR 71.5 lacs
+</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>“We are not necessarily doubting that God will do the best for us; we are wondering how painful the best will turn out to be.”</t>
+          <t xml:space="preserve">
+Toyota Prius  2011 G Touring Selection Leather Package 1.8 for Sale
+</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>C.S. Lewis</t>
+          <t xml:space="preserve">
+                        PKR 43.9 lacs
+</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>“The fear of death follows from the fear of life. A man who lives fully is prepared to die at any time.”</t>
+          <t xml:space="preserve">
+Toyota Aqua  2013 S for Sale
+</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>Mark Twain</t>
+          <t xml:space="preserve">
+                        PKR 32.65 lacs
+</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>“A lie can travel half way around the world while the truth is putting on its shoes.”</t>
+          <t xml:space="preserve">
+Toyota Corolla  2021 Altis X Automatic 1.6 for Sale
+</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>Mark Twain</t>
+          <t xml:space="preserve">
+                        PKR 58 lacs
+</t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>“I believe in Christianity as I believe that the sun has risen: not only because I see it, but because by it I see everything else.”</t>
+          <t xml:space="preserve">
+Toyota Corolla  2022 Altis Grande X CVT-i 1.8 Black Interior for Sale
+</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>C.S. Lewis</t>
+          <t xml:space="preserve">
+                        PKR 68 lacs
+</t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>“The truth." Dumbledore sighed. "It is a beautiful and terrible thing, and should therefore be treated with great caution.”</t>
+          <t xml:space="preserve">
+Toyota Corolla  2018 GLi 1.3 VVTi for Sale
+</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>J.K. Rowling</t>
+          <t xml:space="preserve">
+                        PKR 41 lacs
+</t>
         </is>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>“I'm the one that's got to die when it's time for me to die, so let me live my life the way I want to.”</t>
+          <t xml:space="preserve">
+Toyota B B  2007  for Sale
+</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>Jimi Hendrix</t>
+          <t xml:space="preserve">
+                        PKR 18.5 lacs
+</t>
         </is>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>“To die will be an awfully big adventure.”</t>
+          <t xml:space="preserve">
+Toyota Passo  2011 Plus Hana C for Sale
+</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>J.M. Barrie</t>
+          <t xml:space="preserve">
+                        PKR 23.5 lacs
+</t>
         </is>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>“It takes courage to grow up and become who you really are.”</t>
+          <t xml:space="preserve">
+Toyota Belta  2007 X 1.0 for Sale
+</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>E.E. Cummings</t>
+          <t xml:space="preserve">
+                        PKR 19.5 lacs
+</t>
         </is>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>“But better to get hurt by the truth than comforted with a lie.”</t>
+          <t xml:space="preserve">
+Toyota Prius  2010  for Sale
+</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>Khaled Hosseini</t>
+          <t xml:space="preserve">
+                        PKR 31.25 lacs
+</t>
         </is>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>“You never really understand a person until you consider things from his point of view... Until you climb inside of his skin and walk around in it.”</t>
+          <t xml:space="preserve">
+Toyota Corolla  2012 GLi 1.3 VVTi for Sale
+</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>Harper Lee</t>
+          <t xml:space="preserve">
+                        PKR 22.6 lacs
+</t>
         </is>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>“You have to write the book that wants to be written. And if the book will be too difficult for grown-ups, then you write it for children.”</t>
+          <t xml:space="preserve">
+Toyota Vitz  2018 F 1.0 for Sale
+</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>Madeleine L'Engle</t>
+          <t xml:space="preserve">
+                        PKR 36.5 lacs
+</t>
         </is>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>“Never tell the truth to people who are not worthy of it.”</t>
+          <t xml:space="preserve">
+Toyota Belta  2007 X 1.3 for Sale
+</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>Mark Twain</t>
+          <t xml:space="preserve">
+                        PKR 20.5 lacs
+</t>
         </is>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>“A person's a person, no matter how small.”</t>
+          <t xml:space="preserve">
+Toyota Corolla  2015 GLi Automatic 1.3 VVTi for Sale
+</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>Dr. Seuss</t>
+          <t xml:space="preserve">
+                        PKR 34 lacs
+</t>
         </is>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>“... a mind needs books as a sword needs a whetstone, if it is to keep its edge.”</t>
+          <t xml:space="preserve">
+Toyota Corolla  2005 SE Saloon Automatic for Sale
+</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>George R.R. Martin</t>
+          <t xml:space="preserve">
+                        PKR 16.5 lacs
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Toyota Vitz  2009 F 1.0 for Sale
+</t>
+        </is>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                        PKR 20.7 lacs
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Toyota Hilux  2023 Revo Rocco for Sale
+</t>
+        </is>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                        PKR 1.42 crore
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Toyota Vitz  2013 F Limited 1.0 for Sale
+</t>
+        </is>
+      </c>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                        PKR 23.95 lacs
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Toyota Prius  2011 S 1.5 for Sale
+</t>
+        </is>
+      </c>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                        PKR 29.5 lacs
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Toyota Corolla  1990 SE Limited for Sale
+</t>
+        </is>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                        PKR 19 lacs
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Toyota Corolla  2015 GLi 1.3 VVTi for Sale
+</t>
+        </is>
+      </c>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                        PKR 29.9 lacs
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Toyota Yaris Hatchback  2020  for Sale
+</t>
+        </is>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                        PKR 47 lacs
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Toyota Corolla  2013 GLi 1.3 VVTi for Sale
+</t>
+        </is>
+      </c>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                        PKR 26 lacs
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Toyota Corolla  2015 GLi Automatic 1.3 VVTi for Sale
+</t>
+        </is>
+      </c>
+      <c r="B110" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                        PKR 34.5 lacs
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Toyota Belta  2011 X Business A Package 1.0 for Sale
+</t>
+        </is>
+      </c>
+      <c r="B111" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                        PKR 20.5 lacs
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Toyota Corolla  2020 GLi Automatic 1.3 VVTi for Sale
+</t>
+        </is>
+      </c>
+      <c r="B112" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                        PKR 47.5 lacs
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Toyota Corolla  2020 Altis Grande CVT-i 1.8 for Sale
+</t>
+        </is>
+      </c>
+      <c r="B113" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                        PKR 58.5 lacs
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Toyota C-HR  2018 G-LED for Sale
+</t>
+        </is>
+      </c>
+      <c r="B114" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                        PKR 89 lacs
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Toyota Vitz  2006 iLL 1.0 for Sale
+</t>
+        </is>
+      </c>
+      <c r="B115" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                        PKR 19 lacs
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Toyota Corolla  2021 Altis X Automatic 1.6 for Sale
+</t>
+        </is>
+      </c>
+      <c r="B116" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                        PKR 55.5 lacs
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Toyota Passo  2014 X for Sale
+</t>
+        </is>
+      </c>
+      <c r="B117" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                        PKR 25.5 lacs
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Toyota Hilux  2003 Tiger for Sale
+</t>
+        </is>
+      </c>
+      <c r="B118" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                        PKR 25.5 lacs
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Toyota Corolla 9th Generation 2007 XLi for Sale
+</t>
+        </is>
+      </c>
+      <c r="B119" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                        PKR 19.25 lacs
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Toyota Corolla  2010 GLi 1.3 VVTi for Sale
+</t>
+        </is>
+      </c>
+      <c r="B120" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                        PKR 26.5 lacs
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Toyota Hilux  2013  for Sale
+</t>
+        </is>
+      </c>
+      <c r="B121" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                        PKR 72.5 lacs
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Toyota Vitz  2010 F 1.0 for Sale
+</t>
+        </is>
+      </c>
+      <c r="B122" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                        PKR 19.5 lacs
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Toyota Corolla  2022 Altis 1.6 X CVT-i Special Edition for Sale
+</t>
+        </is>
+      </c>
+      <c r="B123" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                        PKR 66.85 lacs
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Toyota Corolla  2022 Altis 1.6 X CVT-i Special Edition for Sale
+</t>
+        </is>
+      </c>
+      <c r="B124" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                        PKR 69.25 lacs
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Toyota Yaris  2021 ATIV CVT 1.3 for Sale
+</t>
+        </is>
+      </c>
+      <c r="B125" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                        PKR 45 lacs
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Toyota Yaris  2021 GLI MT 1.3 for Sale
+</t>
+        </is>
+      </c>
+      <c r="B126" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                        PKR 36.75 lacs
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Toyota Yaris  2021 ATIV CVT 1.3 for Sale
+</t>
+        </is>
+      </c>
+      <c r="B127" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                        PKR 44 lacs
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Toyota Passo  2009 G 1.0 for Sale
+</t>
+        </is>
+      </c>
+      <c r="B128" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                        PKR 17.6 lacs
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Toyota Yaris  2023 GLI MT 1.3 for Sale
+</t>
+        </is>
+      </c>
+      <c r="B129" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                        PKR 42 lacs
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Toyota Corolla  1995 GLi 1.6 for Sale
+</t>
+        </is>
+      </c>
+      <c r="B130" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                        PKR 8.5 lacs
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Toyota Fortuner  2013 2.7 VVTi for Sale
+</t>
+        </is>
+      </c>
+      <c r="B131" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                        PKR 80 lacs
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Toyota Yaris  2021 GLI CVT 1.3 for Sale
+</t>
+        </is>
+      </c>
+      <c r="B132" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                        PKR 44 lacs
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Toyota Corolla  2022 Altis Grande X CVT-i 1.8 Black Interior for Sale
+</t>
+        </is>
+      </c>
+      <c r="B133" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                        PKR 72 lacs
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Toyota Rush  2006 G A/T for Sale
+</t>
+        </is>
+      </c>
+      <c r="B134" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                        PKR 30 lacs
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Toyota Passo  2007 G 1.0 for Sale
+</t>
+        </is>
+      </c>
+      <c r="B135" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                        PKR 16.7 lacs
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Toyota Corolla  2016  for Sale
+</t>
+        </is>
+      </c>
+      <c r="B136" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                        PKR 35.8 lacs
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Toyota Prius Alpha  2013 G Touring for Sale
+</t>
+        </is>
+      </c>
+      <c r="B137" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                        PKR 42 lacs
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Toyota Vitz  2018 F Safety 1.0 for Sale
+</t>
+        </is>
+      </c>
+      <c r="B138" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                        PKR 39.5 lacs
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Toyota Corolla Axio  2017 Hybrid 1.5 for Sale
+</t>
+        </is>
+      </c>
+      <c r="B139" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                        PKR 75 lacs
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Toyota Vitz  2013 Jewela 1.0 for Sale
+</t>
+        </is>
+      </c>
+      <c r="B140" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                        PKR 25 lacs
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Toyota Yaris Hatchback  2020  for Sale
+</t>
+        </is>
+      </c>
+      <c r="B141" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                        PKR 47 lacs
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Toyota Corolla  2022 Altis X Automatic 1.6 for Sale
+</t>
+        </is>
+      </c>
+      <c r="B142" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                        PKR 68.5 lacs
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Toyota Corolla  2015 GLi Automatic 1.3 VVTi for Sale
+</t>
+        </is>
+      </c>
+      <c r="B143" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                        PKR 33.8 lacs
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Toyota Corona  1990 EX Saloon for Sale
+</t>
+        </is>
+      </c>
+      <c r="B144" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                        PKR 6 lacs
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Toyota Aqua  2015 S for Sale
+</t>
+        </is>
+      </c>
+      <c r="B145" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                        PKR 42.5 lacs
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Toyota Corolla  2020 Altis Automatic 1.6 for Sale
+</t>
+        </is>
+      </c>
+      <c r="B146" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                        PKR 51.5 lacs
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Toyota Belta  2012 X S Package 1.0 for Sale
+</t>
+        </is>
+      </c>
+      <c r="B147" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                        PKR 24.25 lacs
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Toyota Corolla  2020 Altis Grande CVT-i 1.8 for Sale
+</t>
+        </is>
+      </c>
+      <c r="B148" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                        PKR 57.55 lacs
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Toyota Corolla  2015 Altis Grande CVT-i 1.8 for Sale
+</t>
+        </is>
+      </c>
+      <c r="B149" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                        PKR 39.5 lacs
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Toyota Corolla  2020 XLi VVTi for Sale
+</t>
+        </is>
+      </c>
+      <c r="B150" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                        PKR 40 lacs
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Toyota Hilux  2013  for Sale
+</t>
+        </is>
+      </c>
+      <c r="B151" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                        PKR 72 lacs
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Toyota Corolla  2021 Altis X Automatic 1.6 for Sale
+</t>
+        </is>
+      </c>
+      <c r="B152" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                        PKR 56 lacs
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Toyota Corolla  2016 Altis Grande CVT-i 1.8 for Sale
+</t>
+        </is>
+      </c>
+      <c r="B153" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                        PKR 41.35 lacs
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Toyota Belta  2007 X Business A Package 1.0 for Sale
+</t>
+        </is>
+      </c>
+      <c r="B154" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                        PKR 18.5 lacs
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Toyota Prius  2011 S LED Edition 1.8 for Sale
+</t>
+        </is>
+      </c>
+      <c r="B155" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                        PKR 40 lacs
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Toyota Corolla  2017 Altis Automatic 1.6 for Sale
+</t>
+        </is>
+      </c>
+      <c r="B156" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                        PKR 40.95 lacs
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Toyota Corolla  2016 GLi 1.3 VVTi for Sale
+</t>
+        </is>
+      </c>
+      <c r="B157" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                        PKR 31 lacs
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Toyota Corolla  2023 Altis Grande X CVT-i 1.8 Black Interior for Sale
+</t>
+        </is>
+      </c>
+      <c r="B158" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                        PKR 82.75 lacs
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Toyota Vitz  2018 F Safety 1.0 for Sale
+</t>
+        </is>
+      </c>
+      <c r="B159" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                        PKR 42 lacs
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Toyota C-HR  2017 G-LED for Sale
+</t>
+        </is>
+      </c>
+      <c r="B160" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                        PKR 85 lacs
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Toyota Corolla  2018 Altis Grande CVT-i 1.8 for Sale
+</t>
+        </is>
+      </c>
+      <c r="B161" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                        PKR 52.5 lacs
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Toyota Fortuner  2014 2.7 VVTi for Sale
+</t>
+        </is>
+      </c>
+      <c r="B162" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                        PKR 66 lacs
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Toyota Land Cruiser 80 Series 1994 VX 4.5 for Sale
+</t>
+        </is>
+      </c>
+      <c r="B163" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                        PKR 38.5 lacs
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Toyota Corolla  2023 Altis 1.6 X CVT-i Special Edition for Sale
+</t>
+        </is>
+      </c>
+      <c r="B164" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                        PKR 78 lacs
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Toyota Aqua  2014  for Sale
+</t>
+        </is>
+      </c>
+      <c r="B165" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                        PKR 33 lacs
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Toyota Prius  2013  for Sale
+</t>
+        </is>
+      </c>
+      <c r="B166" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                        PKR 45 lacs
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Toyota Corolla  2022 Altis 1.6 X CVT-i for Sale
+</t>
+        </is>
+      </c>
+      <c r="B167" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                        PKR 57.35 lacs
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Toyota Corolla  2016 GLi 1.3 VVTi for Sale
+</t>
+        </is>
+      </c>
+      <c r="B168" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                        PKR 30.5 lacs
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Toyota Allex  2006 1.5 XS for Sale
+</t>
+        </is>
+      </c>
+      <c r="B169" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                        PKR 12.5 lacs
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Toyota Vitz  2014 Jewela 1.0 for Sale
+</t>
+        </is>
+      </c>
+      <c r="B170" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                        PKR 34.5 lacs
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Toyota Surf  2000 SSR-X 2.7 for Sale
+</t>
+        </is>
+      </c>
+      <c r="B171" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                        PKR 47 lacs
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Toyota Yaris  2021 ATIV X CVT 1.5 for Sale
+</t>
+        </is>
+      </c>
+      <c r="B172" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                        PKR 44 lacs
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Toyota Yaris  2020 ATIV X CVT 1.5 for Sale
+</t>
+        </is>
+      </c>
+      <c r="B173" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                        PKR 43.5 lacs
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Toyota Corolla  2016 Altis Automatic 1.6 for Sale
+</t>
+        </is>
+      </c>
+      <c r="B174" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                        PKR 42.5 lacs
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Toyota Corolla  2022 Altis 1.6 X CVT-i for Sale
+</t>
+        </is>
+      </c>
+      <c r="B175" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                        PKR 57.4 lacs
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Toyota Harrier  2002 2.0 LUXURY for Sale
+</t>
+        </is>
+      </c>
+      <c r="B176" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                        PKR 25 lacs
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Toyota Corolla  2022 Altis X Automatic 1.6 for Sale
+</t>
+        </is>
+      </c>
+      <c r="B177" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                        PKR 62 lacs
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Toyota Vitz  2006 U 1.0 for Sale
+</t>
+        </is>
+      </c>
+      <c r="B178" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                        PKR 19 lacs
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Toyota Vitz  2014 F Limited 1.0 for Sale
+</t>
+        </is>
+      </c>
+      <c r="B179" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                        PKR 27.6 lacs
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Toyota Voxy  2018  for Sale
+</t>
+        </is>
+      </c>
+      <c r="B180" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                        PKR 78.5 lacs
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Toyota Starlet  1981 1.2 for Sale
+</t>
+        </is>
+      </c>
+      <c r="B181" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                        PKR 6.5 lacs
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="182">
+      <c r="A182" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Toyota Aqua  2012 G for Sale
+</t>
+        </is>
+      </c>
+      <c r="B182" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                        PKR 31.5 lacs
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="183">
+      <c r="A183" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Toyota Vitz  2019 F 1.0 for Sale
+</t>
+        </is>
+      </c>
+      <c r="B183" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                        PKR 40.45 lacs
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="184">
+      <c r="A184" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Toyota Belta  2009 X 1.3 for Sale
+</t>
+        </is>
+      </c>
+      <c r="B184" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                        PKR 20.75 lacs
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="185">
+      <c r="A185" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Toyota Corolla  2016 GLi Automatic 1.3 VVTi for Sale
+</t>
+        </is>
+      </c>
+      <c r="B185" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                        PKR 34.75 lacs
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="186">
+      <c r="A186" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Toyota Crown  1997 Royal Saloon G for Sale
+</t>
+        </is>
+      </c>
+      <c r="B186" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                        PKR 35 lacs
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="187">
+      <c r="A187" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Toyota Vitz  2012 F Smile Edition 1.0 for Sale
+</t>
+        </is>
+      </c>
+      <c r="B187" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                        PKR 23.5 lacs
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="188">
+      <c r="A188" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Toyota Corolla  1993  for Sale
+</t>
+        </is>
+      </c>
+      <c r="B188" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                        PKR 5.6 lacs
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="189">
+      <c r="A189" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Toyota Corolla  2022 Altis 1.6 X CVT-i for Sale
+</t>
+        </is>
+      </c>
+      <c r="B189" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                        PKR 63 lacs
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="190">
+      <c r="A190" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Toyota Corolla Indus 2001 2.0D Limited for Sale
+</t>
+        </is>
+      </c>
+      <c r="B190" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                        PKR 9.8 lacs
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="191">
+      <c r="A191" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Toyota Corolla  2013 XLi VVTi Limited Edition for Sale
+</t>
+        </is>
+      </c>
+      <c r="B191" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                        PKR 19 lacs
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="192">
+      <c r="A192" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Toyota Corolla  2021 Altis X Automatic 1.6 for Sale
+</t>
+        </is>
+      </c>
+      <c r="B192" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                        PKR 58.5 lacs
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="193">
+      <c r="A193" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Toyota Prius  2012 S 1.8 for Sale
+</t>
+        </is>
+      </c>
+      <c r="B193" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                        PKR 39 lacs
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="194">
+      <c r="A194" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Toyota Crown  1996 Royal Saloon G for Sale
+</t>
+        </is>
+      </c>
+      <c r="B194" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                        PKR 32 lacs
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="195">
+      <c r="A195" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Toyota Prado 90 Series 1998 RZ 3.4 (3-Door) for Sale
+</t>
+        </is>
+      </c>
+      <c r="B195" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                        PKR 36.5 lacs
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="196">
+      <c r="A196" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Toyota Corolla  2022 Altis 1.6 X CVT-i for Sale
+</t>
+        </is>
+      </c>
+      <c r="B196" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                        PKR 65 lacs
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="197">
+      <c r="A197" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Toyota Vitz  2011 F 1.0 for Sale
+</t>
+        </is>
+      </c>
+      <c r="B197" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                        PKR 23 lacs
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="198">
+      <c r="A198" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Toyota Corolla  2018 Altis Automatic 1.6 for Sale
+</t>
+        </is>
+      </c>
+      <c r="B198" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                        PKR 41.5 lacs
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="199">
+      <c r="A199" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Toyota Corolla  2023 Altis Grande X CVT-i 1.8 Black Interior for Sale
+</t>
+        </is>
+      </c>
+      <c r="B199" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                        PKR 82 lacs
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="200">
+      <c r="A200" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Toyota Fortuner  2022 Legender  for Sale
+</t>
+        </is>
+      </c>
+      <c r="B200" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                        PKR 1.88 crore
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="201">
+      <c r="A201" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Toyota Corolla  1990 SE Limited for Sale
+</t>
+        </is>
+      </c>
+      <c r="B201" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                        PKR 11.5 lacs
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="202">
+      <c r="A202" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Toyota Passo  2007  for Sale
+</t>
+        </is>
+      </c>
+      <c r="B202" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                        PKR 17 lacs
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="203">
+      <c r="A203" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Toyota Vitz  2012 F 1.0 for Sale
+</t>
+        </is>
+      </c>
+      <c r="B203" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                        PKR 24.75 lacs
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="204">
+      <c r="A204" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Toyota Corolla  2017 Altis Grande CVT-i 1.8 for Sale
+</t>
+        </is>
+      </c>
+      <c r="B204" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                        PKR 48.75 lacs
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="205">
+      <c r="A205" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Toyota Yaris  2021 ATIV MT 1.3 for Sale
+</t>
+        </is>
+      </c>
+      <c r="B205" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                        PKR 41.5 lacs
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="206">
+      <c r="A206" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Toyota Vitz  2004 FL 1.0 for Sale
+</t>
+        </is>
+      </c>
+      <c r="B206" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                        PKR 17.5 lacs
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="207">
+      <c r="A207" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Toyota Corolla  2018 GLi Automatic 1.3 VVTi for Sale
+</t>
+        </is>
+      </c>
+      <c r="B207" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                        PKR 41.5 lacs
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="208">
+      <c r="A208" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Toyota Yaris  2021 ATIV X CVT 1.5 for Sale
+</t>
+        </is>
+      </c>
+      <c r="B208" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                        PKR 44.5 lacs
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="209">
+      <c r="A209" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Toyota Passo  2012 X for Sale
+</t>
+        </is>
+      </c>
+      <c r="B209" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                        PKR 23.75 lacs
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="210">
+      <c r="A210" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Toyota Passo  2013  for Sale
+</t>
+        </is>
+      </c>
+      <c r="B210" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                        PKR 23 lacs
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="211">
+      <c r="A211" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Toyota Platz  2000 F 1.0 for Sale
+</t>
+        </is>
+      </c>
+      <c r="B211" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                        PKR 12.5 lacs
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="212">
+      <c r="A212" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Toyota Yaris  2021 ATIV CVT 1.3 for Sale
+</t>
+        </is>
+      </c>
+      <c r="B212" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                        PKR 42 lacs
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="213">
+      <c r="A213" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Toyota Corolla  2019 GLi 1.3 VVTi for Sale
+</t>
+        </is>
+      </c>
+      <c r="B213" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                        PKR 41 lacs
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="214">
+      <c r="A214" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Toyota Corolla  2005 Altis Automatic 1.8 for Sale
+</t>
+        </is>
+      </c>
+      <c r="B214" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                        PKR 16.75 lacs
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="215">
+      <c r="A215" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Toyota Vitz  2014 Jewela 1.0 for Sale
+</t>
+        </is>
+      </c>
+      <c r="B215" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                        PKR 28.5 lacs
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="216">
+      <c r="A216" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Toyota Fortuner  2022 Legender  for Sale
+</t>
+        </is>
+      </c>
+      <c r="B216" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                        PKR 1.92 crore
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="217">
+      <c r="A217" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Toyota Corolla  2020 Altis Automatic 1.6 for Sale
+</t>
+        </is>
+      </c>
+      <c r="B217" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                        PKR 53.75 lacs
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="218">
+      <c r="A218" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Toyota Hilux  2008 D-4D Automatic for Sale
+</t>
+        </is>
+      </c>
+      <c r="B218" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                        PKR 44.9 lacs
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="219">
+      <c r="A219" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Toyota Corolla  2018 GLi Automatic 1.3 VVTi for Sale
+</t>
+        </is>
+      </c>
+      <c r="B219" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                        PKR 40 lacs
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="220">
+      <c r="A220" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Toyota Land Cruiser  2017 ZX G-Frontier for Sale
+</t>
+        </is>
+      </c>
+      <c r="B220" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                        PKR 4.55 crore
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="221">
+      <c r="A221" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Toyota Prado  2008 TX 2.7 for Sale
+</t>
+        </is>
+      </c>
+      <c r="B221" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                        PKR 1.05 crore
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="222">
+      <c r="A222" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Toyota Passo  2018 X G Package for Sale
+</t>
+        </is>
+      </c>
+      <c r="B222" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                        PKR 36 lacs
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="223">
+      <c r="A223" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Toyota Yaris  2021 GLI CVT 1.3 for Sale
+</t>
+        </is>
+      </c>
+      <c r="B223" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                        PKR 44.5 lacs
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="224">
+      <c r="A224" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Toyota Starlet  1978 1.0 for Sale
+</t>
+        </is>
+      </c>
+      <c r="B224" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                        PKR 2.8 lacs
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="225">
+      <c r="A225" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Toyota Corolla  2021 Altis X Automatic 1.6 for Sale
+</t>
+        </is>
+      </c>
+      <c r="B225" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                        PKR 54.3 lacs
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="226">
+      <c r="A226" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Toyota Corolla  2001  for Sale
+</t>
+        </is>
+      </c>
+      <c r="B226" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                        PKR 25.75 lacs
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="227">
+      <c r="A227" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Toyota Prius Alpha  2013 S Touring for Sale
+</t>
+        </is>
+      </c>
+      <c r="B227" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                        PKR 42 lacs
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="228">
+      <c r="A228" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Toyota Vitz  2012  for Sale
+</t>
+        </is>
+      </c>
+      <c r="B228" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                        PKR 23.3 lacs
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="229">
+      <c r="A229" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Toyota Belta  2007 X Business A Package 1.3 for Sale
+</t>
+        </is>
+      </c>
+      <c r="B229" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                        PKR 21 lacs
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="230">
+      <c r="A230" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Toyota Corolla  2009 GLi 1.3 VVTi for Sale
+</t>
+        </is>
+      </c>
+      <c r="B230" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                        PKR 19 lacs
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="231">
+      <c r="A231" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Toyota Aqua  2018 S for Sale
+</t>
+        </is>
+      </c>
+      <c r="B231" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                        PKR 52 lacs
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="232">
+      <c r="A232" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Toyota Corolla Axio  2016 Hybrid 1.5 for Sale
+</t>
+        </is>
+      </c>
+      <c r="B232" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                        PKR 52 lacs
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="233">
+      <c r="A233" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Toyota Vitz  2001 F 1.0 for Sale
+</t>
+        </is>
+      </c>
+      <c r="B233" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                        PKR 13.5 lacs
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="234">
+      <c r="A234" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Toyota Hilux  2002  for Sale
+</t>
+        </is>
+      </c>
+      <c r="B234" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                        PKR 26.5 lacs
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="235">
+      <c r="A235" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Toyota Corolla  2022 Altis 1.6 X CVT-i for Sale
+</t>
+        </is>
+      </c>
+      <c r="B235" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                        PKR 59.5 lacs
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="236">
+      <c r="A236" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Toyota Passo  2018 X S  for Sale
+</t>
+        </is>
+      </c>
+      <c r="B236" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                        PKR 34.65 lacs
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="237">
+      <c r="A237" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Toyota Vitz  2012 F Limited II 1.0 for Sale
+</t>
+        </is>
+      </c>
+      <c r="B237" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                        PKR 23.2 lacs
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="238">
+      <c r="A238" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Toyota Aqua  2012 S for Sale
+</t>
+        </is>
+      </c>
+      <c r="B238" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                        PKR 30 lacs
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="239">
+      <c r="A239" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Toyota Corolla Indus 1994 SE Limited for Sale
+</t>
+        </is>
+      </c>
+      <c r="B239" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                        PKR 9 lacs
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="240">
+      <c r="A240" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Toyota Corolla  2004 GLi 1.3 for Sale
+</t>
+        </is>
+      </c>
+      <c r="B240" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                        PKR 13.5 lacs
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="241">
+      <c r="A241" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Toyota Corolla  2018 Altis Grande CVT-i 1.8 for Sale
+</t>
+        </is>
+      </c>
+      <c r="B241" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                        PKR 52 lacs
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="242">
+      <c r="A242" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Toyota Corolla  1987 DX Saloon for Sale
+</t>
+        </is>
+      </c>
+      <c r="B242" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                        PKR 2.59 lacs
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="243">
+      <c r="A243" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Toyota Yaris  2010  for Sale
+</t>
+        </is>
+      </c>
+      <c r="B243" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                        PKR 21 lacs
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="244">
+      <c r="A244" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Toyota Premio  2002 X 1.8 for Sale
+</t>
+        </is>
+      </c>
+      <c r="B244" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                        PKR 22 lacs
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="245">
+      <c r="A245" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Toyota Corolla  2018 GLi 1.3 VVTi for Sale
+</t>
+        </is>
+      </c>
+      <c r="B245" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                        PKR 37.5 lacs
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="246">
+      <c r="A246" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Toyota Corolla 9th Generation 2007 Altis 1.8 for Sale
+</t>
+        </is>
+      </c>
+      <c r="B246" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                        PKR 14.75 lacs
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="247">
+      <c r="A247" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Toyota Corolla  2019 GLi Automatic 1.3 VVTi for Sale
+</t>
+        </is>
+      </c>
+      <c r="B247" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                        PKR 43 lacs
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="248">
+      <c r="A248" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Toyota Vitz  2000  for Sale
+</t>
+        </is>
+      </c>
+      <c r="B248" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                        PKR 11.95 lacs
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="249">
+      <c r="A249" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Toyota Aqua  2017 S for Sale
+</t>
+        </is>
+      </c>
+      <c r="B249" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                        PKR 55 lacs
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="250">
+      <c r="A250" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Toyota Prius  2010  for Sale
+</t>
+        </is>
+      </c>
+      <c r="B250" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                        PKR 33 lacs
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="251">
+      <c r="A251" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Toyota Corolla Axio  2007 X 1.5 for Sale
+</t>
+        </is>
+      </c>
+      <c r="B251" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                        PKR 31.5 lacs
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="252">
+      <c r="A252" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Toyota Corolla  2022 Altis X Automatic 1.6 for Sale
+</t>
+        </is>
+      </c>
+      <c r="B252" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                        PKR 65 lacs
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="253">
+      <c r="A253" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Toyota Corolla Axio  2013 Hybrid 1.5 for Sale
+</t>
+        </is>
+      </c>
+      <c r="B253" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                        PKR 40 lacs
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="254">
+      <c r="A254" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Toyota Corolla  2022 Altis X Automatic 1.6 for Sale
+</t>
+        </is>
+      </c>
+      <c r="B254" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                        PKR 64.5 lacs
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="255">
+      <c r="A255" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Toyota Platz  1999 F 1.0 for Sale
+</t>
+        </is>
+      </c>
+      <c r="B255" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                        PKR 10.3 lacs
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="256">
+      <c r="A256" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Toyota Corolla  2013 XLi VVTi for Sale
+</t>
+        </is>
+      </c>
+      <c r="B256" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                        PKR 20.75 lacs
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="257">
+      <c r="A257" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Toyota Corolla  2022 Altis 1.6 X CVT-i Special Edition for Sale
+</t>
+        </is>
+      </c>
+      <c r="B257" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                        PKR 65.1 lacs
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="258">
+      <c r="A258" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Toyota Corolla  2006 2.0D for Sale
+</t>
+        </is>
+      </c>
+      <c r="B258" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                        PKR 17.5 lacs
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="259">
+      <c r="A259" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Toyota Vitz  2009 F 1.3 for Sale
+</t>
+        </is>
+      </c>
+      <c r="B259" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                        PKR 23 lacs
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="260">
+      <c r="A260" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Toyota Platz  1999  for Sale
+</t>
+        </is>
+      </c>
+      <c r="B260" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                        PKR 10.3 lacs
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="261">
+      <c r="A261" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+Toyota Corolla  2022 Altis X Automatic 1.6 for Sale
+</t>
+        </is>
+      </c>
+      <c r="B261" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+                        PKR 57.75 lacs
+</t>
         </is>
       </c>
     </row>

</xml_diff>